<commit_message>
Add excel into module
</commit_message>
<xml_diff>
--- a/test_module3.xlsx
+++ b/test_module3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2379c53a403574eb/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85B3D73F-EDD7-496C-8768-9C12DB7DD413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{85B3D73F-EDD7-496C-8768-9C12DB7DD413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7662146-64BD-4C70-AF3B-236089F6F00B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{EA940391-3A66-4BAB-8A46-F9A68201311D}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{EA940391-3A66-4BAB-8A46-F9A68201311D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Cashflow</t>
+  </si>
+  <si>
+    <t>Discount factor</t>
+  </si>
+  <si>
+    <t>NPV</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -66,8 +83,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,25 +422,167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCE6D1C-BAC9-40A1-8D3B-B5380BBC691B}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>2025</v>
+      </c>
+      <c r="C1">
+        <f>B1+1</f>
+        <v>2026</v>
+      </c>
+      <c r="D1">
+        <f t="shared" ref="D1:L1" si="0">C1+1</f>
+        <v>2027</v>
+      </c>
+      <c r="E1">
+        <f t="shared" si="0"/>
+        <v>2028</v>
+      </c>
+      <c r="F1">
+        <f t="shared" si="0"/>
+        <v>2029</v>
+      </c>
+      <c r="G1">
+        <f t="shared" si="0"/>
+        <v>2030</v>
+      </c>
+      <c r="H1">
+        <f t="shared" si="0"/>
+        <v>2031</v>
+      </c>
+      <c r="I1">
+        <f t="shared" si="0"/>
+        <v>2032</v>
+      </c>
+      <c r="J1">
+        <f t="shared" si="0"/>
+        <v>2033</v>
+      </c>
+      <c r="K1">
+        <f t="shared" si="0"/>
+        <v>2034</v>
+      </c>
+      <c r="L1">
+        <f t="shared" si="0"/>
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <f ca="1">10000*RAND()</f>
+        <v>929.69829601073366</v>
+      </c>
+      <c r="C2" s="1">
+        <f t="shared" ref="C2:L2" ca="1" si="1">10000*RAND()</f>
+        <v>5276.973471737113</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>6653.6251517768287</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>7650.4213518578599</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>2210.7699776881072</v>
+      </c>
+      <c r="G2" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>7197.198337833046</v>
+      </c>
+      <c r="H2" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>6554.0280029374735</v>
+      </c>
+      <c r="I2" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>7569.64589734334</v>
+      </c>
+      <c r="J2" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>6684.9898908502246</v>
+      </c>
+      <c r="K2" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>1393.1902882613579</v>
+      </c>
+      <c r="L2" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>1157.5211977022516</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B1">
+      <c r="B3" s="2">
+        <f>1/(1.05)^(B1-$B$1+1)</f>
+        <v>0.95238095238095233</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:L3" si="2">1/(1.05)^(C1-$B$1+1)</f>
+        <v>0.90702947845804982</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" si="2"/>
+        <v>0.86383759853147601</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" si="2"/>
+        <v>0.82270247479188197</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" si="2"/>
+        <v>0.78352616646845896</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" si="2"/>
+        <v>0.74621539663662761</v>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" si="2"/>
+        <v>0.71068133013012147</v>
+      </c>
+      <c r="I3" s="2">
+        <f t="shared" si="2"/>
+        <v>0.67683936202868722</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" si="2"/>
+        <v>0.64460891621779726</v>
+      </c>
+      <c r="K3" s="2">
+        <f t="shared" si="2"/>
+        <v>0.61391325354075932</v>
+      </c>
+      <c r="L3" s="2">
+        <f t="shared" si="2"/>
+        <v>0.5846792890864374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B2">
-        <v>4</v>
+      <c r="B5" s="3">
+        <f ca="1">SUMPRODUCT(B2:L2,B3:L3)</f>
+        <v>40438.866315291511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>